<commit_message>
pv forecast on the go
</commit_message>
<xml_diff>
--- a/cosimulation/static/demo/0_pv_and_load_forecast/pv_forecast.xlsx
+++ b/cosimulation/static/demo/0_pv_and_load_forecast/pv_forecast.xlsx
@@ -24,24 +24,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>NARX_NET_FILE</t>
-  </si>
-  <si>
-    <t>independent_pv_input</t>
-  </si>
-  <si>
-    <t>independent_inputs.csv</t>
-  </si>
-  <si>
-    <t>FANN_NET_FILE</t>
-  </si>
-  <si>
-    <t>narx-2-1-65.net</t>
-  </si>
-  <si>
-    <t>fann-2-1-65.net</t>
+    <t>zip_code</t>
   </si>
 </sst>
 </file>
@@ -368,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -380,26 +365,14 @@
     <col min="3" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>94553</v>
       </c>
     </row>
   </sheetData>

</xml_diff>